<commit_message>
Journal de travail mise à jour.
</commit_message>
<xml_diff>
--- a/Journaux_de_travail/Christopher.xlsx
+++ b/Journaux_de_travail/Christopher.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Journal de travail</t>
   </si>
@@ -38,6 +38,30 @@
   </si>
   <si>
     <t xml:space="preserve">Découverte du projet, initialisation des outils collaboratifs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BD : Modèle conceptuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liste des fonctionnalités</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organisation du serveur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagramme de classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paramétrage de l’ORM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Architecture client-serveur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Révision diagramme de classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BD : Modèle logique</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -291,7 +315,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -336,45 +360,93 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="n">
+        <v>43001</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="n">
+        <v>43002</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="n">
+        <v>43009</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="n">
+        <v>43011</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="8" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="n">
+        <v>43011</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="8" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="n">
+        <v>43017</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="n">
+        <v>43018</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="n">
+        <v>43018</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="8" t="n">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6"/>
@@ -468,11 +540,11 @@
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="9" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C32" s="10" t="n">
         <f aca="false">SUM(C5:C31)</f>
-        <v>3.5</v>
+        <v>24.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected Rack, Slot with DB. Added methood to Bag. Created a ChallengeFactory to facilitate creation of a Challenge. Ignore some field with JackSON to stop recursive marshalling.
</commit_message>
<xml_diff>
--- a/Journaux_de_travail/Christopher.xlsx
+++ b/Journaux_de_travail/Christopher.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t xml:space="preserve">Journal de travail</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">BD : Modèle logique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BD : Hibernate</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -315,7 +318,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -448,15 +451,27 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="n">
+        <v>43031</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="8" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="n">
+        <v>43032</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="8" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6"/>
@@ -540,11 +555,11 @@
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C32" s="10" t="n">
         <f aca="false">SUM(C5:C31)</f>
-        <v>24.5</v>
+        <v>36.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>